<commit_message>
map upper I-5 and I-10
</commit_message>
<xml_diff>
--- a/led_locations.xlsx
+++ b/led_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D54FEC-7863-4F6F-8156-9BB5C34D8B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6E55C0-706A-47F0-8EBB-C26D7C352AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="479">
   <si>
     <t>LED Number</t>
   </si>
@@ -1213,6 +1213,255 @@
   </si>
   <si>
     <t>C6wpiRhDkAEYGPoZAH8BDA==</t>
+  </si>
+  <si>
+    <t>C6uZ3BiUkQEOqxh05FABHQ==</t>
+  </si>
+  <si>
+    <t>C6uk2RiIWQEer+aoHJYBCw==</t>
+  </si>
+  <si>
+    <t>C6ulQRiHqQENEgJp/MQBHQ==</t>
+  </si>
+  <si>
+    <t>C6umuxiBIgEAUPv2D3sBDg==</t>
+  </si>
+  <si>
+    <t>C6ummhiASwEPJQYK+nUBGg==</t>
+  </si>
+  <si>
+    <t>C6unoRh+wgEcG/4TBRgBEA==</t>
+  </si>
+  <si>
+    <t>C6upaxh9tgEKFgQU/O8BGw==</t>
+  </si>
+  <si>
+    <t>C6usRBh7LwEdN/YOB6sBDA==</t>
+  </si>
+  <si>
+    <t>C6us6hh52gENHgKV+jIBHg==</t>
+  </si>
+  <si>
+    <t>C6utyhh4BgEeI/y6BskBDg==</t>
+  </si>
+  <si>
+    <t>C6uuHhh3JQEOGgGh+rEBHw==</t>
+  </si>
+  <si>
+    <t>C6uupBh15AEfF/4sBJIBDg==</t>
+  </si>
+  <si>
+    <t>C6uu4Bh0rAEPIQLt+aoBHQ==</t>
+  </si>
+  <si>
+    <t>C6uvlRhy6gEeIP37BmUBDg==</t>
+  </si>
+  <si>
+    <t>C6uwPRhxuAENIQOG+dwBHQ==</t>
+  </si>
+  <si>
+    <t>C6uxghhv/gEdIvveBkUBDg==</t>
+  </si>
+  <si>
+    <t>C6ux4Rhu2wENZxNp8z8BHQ==</t>
+  </si>
+  <si>
+    <t>C6u5EBhrDQEaV+/KCpkBDQ==</t>
+  </si>
+  <si>
+    <t>C6u67Rho6gENKQb5+eYBHQ==</t>
+  </si>
+  <si>
+    <t>C6u8UxhoBwEbK/kABn4BCg==</t>
+  </si>
+  <si>
+    <t>C6u8wBhnqgEMDgIx/cMBHA==</t>
+  </si>
+  <si>
+    <t>C6u/DxhlJwEcJvojBisBCw==</t>
+  </si>
+  <si>
+    <t>C6u+LRhmEgENGAPD+/gBHA==</t>
+  </si>
+  <si>
+    <t>C6vAgxhjqQEcE/zhAzQBDA==</t>
+  </si>
+  <si>
+    <t>C6vCbhhhxwELJwYE+aIBHA==</t>
+  </si>
+  <si>
+    <t>C6vD1BhgbwEdLPjiBusBDA==</t>
+  </si>
+  <si>
+    <t>C6vFPBhezwEMGQOk+68BHA==</t>
+  </si>
+  <si>
+    <t>C6vGjBhdUAEdD/3wApIBDA==</t>
+  </si>
+  <si>
+    <t>C6vIJRhbpgEMCwHo/jIBHA==</t>
+  </si>
+  <si>
+    <t>C6vLHRhY6wEcPPY0CW4BDQ==</t>
+  </si>
+  <si>
+    <t>C6vKURhZmwEMHAUF/AEBGQ==</t>
+  </si>
+  <si>
+    <t>C6vMqBhXvgEIDgOX/2sBGQ==</t>
+  </si>
+  <si>
+    <t>C6vPgRhXDgEaGfoTAYcBCQ==</t>
+  </si>
+  <si>
+    <t>C6vRiBhWxAEHDQLe/xABHA==</t>
+  </si>
+  <si>
+    <t>C6vWwhhUoQEbF/uXAr8BGCf2/QHRAQg=</t>
+  </si>
+  <si>
+    <t>C6vUnBhV4gEICgJc/18BGw==</t>
+  </si>
+  <si>
+    <t>C6vXshhTxgEMMwhJ+AcBGw==</t>
+  </si>
+  <si>
+    <t>C6vY1BhSXQEdHfuPBN0BDA==</t>
+  </si>
+  <si>
+    <t>C6vdXRhOtgENEQML/YABHQ==</t>
+  </si>
+  <si>
+    <t>C6vdxRhOWAEcE/ysAtIBDA==</t>
+  </si>
+  <si>
+    <t>C6veyBhNiwENEQJK/PgBGw==</t>
+  </si>
+  <si>
+    <t>C6vfBBhNBgEeEv1TAtUBCw==</t>
+  </si>
+  <si>
+    <t>C6vhOxhLDQENHwUz+2ABHQ==</t>
+  </si>
+  <si>
+    <t>C6viaRhJmwEbHvt3BNEBCw==</t>
+  </si>
+  <si>
+    <t>C6vjpxhI5QEMEgEd/GEBHg==</t>
+  </si>
+  <si>
+    <t>C6vkIRhHmwEfCP+VAbABDw==</t>
+  </si>
+  <si>
+    <t>C6vkLBhHNQEOLgMv9sUBHg==</t>
+  </si>
+  <si>
+    <t>C6vlBhhEjgEeIP4WBo0BDw==</t>
+  </si>
+  <si>
+    <t>C6vmxBhBrQELEQOe/f4BGw==</t>
+  </si>
+  <si>
+    <t>C6vneRhBUQEaEfzGAlQBDQ==</t>
+  </si>
+  <si>
+    <t>C6vpexg/5QENFAMK/KQBHA==</t>
+  </si>
+  <si>
+    <t>C6vqUBg++gEcGPwAA+ABCw==</t>
+  </si>
+  <si>
+    <t>C6vrkRg9tAELEwPk/ZkBGQ==</t>
+  </si>
+  <si>
+    <t>C6vtqRg8iAEZEPy5AdYBCw==</t>
+  </si>
+  <si>
+    <t>C6vu0Rg7eQEQHgGM+fUBHg==</t>
+  </si>
+  <si>
+    <t>C6vvoRg4gQEeGv5NBUEBDw==</t>
+  </si>
+  <si>
+    <t>I-10</t>
+  </si>
+  <si>
+    <t>C6vy8Bg3mAEILgrvAl4BGA==</t>
+  </si>
+  <si>
+    <t>C6v0jRg3mAEYEPwDABMBBw==</t>
+  </si>
+  <si>
+    <t>C6v4CRg4swEIEAOjAOwBFQ==</t>
+  </si>
+  <si>
+    <t>C6v5Dxg4ygEUGfon/rIBBQ==</t>
+  </si>
+  <si>
+    <t>C6v7kxg6GwEEGwaHANkBFw==</t>
+  </si>
+  <si>
+    <t>C6v+ARg6jgEYGfoc/tYBBQ==</t>
+  </si>
+  <si>
+    <t>C6v+nhg6gQEIEQRKAA4BGA==</t>
+  </si>
+  <si>
+    <t>C6wAFxg6lQEYEvuG//IBCA==</t>
+  </si>
+  <si>
+    <t>C6wE8hg6lAEIDQNvAAoBGA==</t>
+  </si>
+  <si>
+    <t>C6wF6Rg6pwEXEfu7AAEBCA==</t>
+  </si>
+  <si>
+    <t>C6wH9Bg6nQEIGAX5ABYBGA==</t>
+  </si>
+  <si>
+    <t>C6wJFBg6sQEXDfy6//YBCA==</t>
+  </si>
+  <si>
+    <t>C6wL2xg6uwEYGPoJ/+oBCA==</t>
+  </si>
+  <si>
+    <t>C6wPvBg57gEIMwxS/l4BFw==</t>
+  </si>
+  <si>
+    <t>C6wQ7Rg55wEYFvp+ALUBCg==</t>
+  </si>
+  <si>
+    <t>C6wWGRg5TAEXEPwJACUBCQ==</t>
+  </si>
+  <si>
+    <t>C6wXZhg5bAEGCwLuAGkBFw==</t>
+  </si>
+  <si>
+    <t>C6wZxRg5yQEXDvx6/4cBBw==</t>
+  </si>
+  <si>
+    <t>C6wadhg51gEHIQhHARQBFw==</t>
+  </si>
+  <si>
+    <t>C6wgaRg6lwEXF/pT/2YBBw==</t>
+  </si>
+  <si>
+    <t>C6whXBg6qQEHEAQAAAgBGA==</t>
+  </si>
+  <si>
+    <t>C6wjcRg6tAEYEPv3AAQBBw==</t>
+  </si>
+  <si>
+    <t>C6wlAxg6pwEIGwbe//MBGA==</t>
+  </si>
+  <si>
+    <t>C6wm/Rg6rAEYHvhjABEBCA==</t>
+  </si>
+  <si>
+    <t>C6woNhg6oQEIGQZj/+wBGA==</t>
+  </si>
+  <si>
+    <t>C6wqXBg6pQEYHfjFAA4BCA==</t>
   </si>
 </sst>
 </file>
@@ -1559,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H471"/>
+  <dimension ref="A1:H567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A433" workbookViewId="0">
-      <selection activeCell="D472" sqref="D472"/>
+    <sheetView tabSelected="1" topLeftCell="A520" workbookViewId="0">
+      <selection activeCell="E567" sqref="E567"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12741,6 +12990,2352 @@
         <v>13</v>
       </c>
     </row>
+    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A472" s="3">
+        <v>118</v>
+      </c>
+      <c r="B472" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C472" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D472" s="2">
+        <v>34.562778000000002</v>
+      </c>
+      <c r="E472" s="2">
+        <v>-118.683605</v>
+      </c>
+      <c r="F472" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G472">
+        <v>72</v>
+      </c>
+      <c r="H472" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A473" s="3">
+        <v>119</v>
+      </c>
+      <c r="B473" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C473" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H473" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A474" s="3">
+        <v>120</v>
+      </c>
+      <c r="B474" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C474" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H474" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A475" s="3">
+        <v>121</v>
+      </c>
+      <c r="B475" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C475" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H475" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A476" s="3">
+        <v>118</v>
+      </c>
+      <c r="B476" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C476" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D476" s="2">
+        <v>34.563246999999997</v>
+      </c>
+      <c r="E476" s="2">
+        <v>-118.682947</v>
+      </c>
+      <c r="F476" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="G476">
+        <v>64</v>
+      </c>
+      <c r="H476" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A477" s="3">
+        <v>119</v>
+      </c>
+      <c r="B477" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C477" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H477" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="478" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A478" s="3">
+        <v>120</v>
+      </c>
+      <c r="B478" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C478" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H478" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="479" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A479" s="3">
+        <v>121</v>
+      </c>
+      <c r="B479" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C479" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H479" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A480" s="3">
+        <v>122</v>
+      </c>
+      <c r="B480" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C480" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D480" s="2">
+        <v>34.491003999999997</v>
+      </c>
+      <c r="E480" s="2">
+        <v>-118.620514</v>
+      </c>
+      <c r="F480" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G480">
+        <v>73</v>
+      </c>
+      <c r="H480" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="481" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A481" s="3">
+        <v>122</v>
+      </c>
+      <c r="B481" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C481" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D481" s="2">
+        <v>34.491188000000001</v>
+      </c>
+      <c r="E481" s="2">
+        <v>-118.62002200000001</v>
+      </c>
+      <c r="F481" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G481">
+        <v>72</v>
+      </c>
+      <c r="H481" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="482" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A482" s="3">
+        <v>123</v>
+      </c>
+      <c r="B482" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C482" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H482" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A483" s="3">
+        <v>124</v>
+      </c>
+      <c r="B483" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C483" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H483" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="484" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A484" s="3">
+        <v>125</v>
+      </c>
+      <c r="B484" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C484" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D484" s="2">
+        <v>34.449930000000002</v>
+      </c>
+      <c r="E484" s="2">
+        <v>-118.61372799999999</v>
+      </c>
+      <c r="F484" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G484">
+        <v>70</v>
+      </c>
+      <c r="H484" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="485" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A485" s="3">
+        <v>125</v>
+      </c>
+      <c r="B485" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C485" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D485" s="2">
+        <v>34.450118000000003</v>
+      </c>
+      <c r="E485" s="2">
+        <v>-118.613421</v>
+      </c>
+      <c r="F485" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G485">
+        <v>71</v>
+      </c>
+      <c r="H485" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="486" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A486" s="3">
+        <v>126</v>
+      </c>
+      <c r="B486" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C486" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D486" s="2">
+        <v>34.438529000000003</v>
+      </c>
+      <c r="E486" s="2">
+        <v>-118.5972</v>
+      </c>
+      <c r="F486" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="G486">
+        <v>68</v>
+      </c>
+      <c r="H486" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="487" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A487" s="3">
+        <v>126</v>
+      </c>
+      <c r="B487" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C487" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D487" s="2">
+        <v>34.438822000000002</v>
+      </c>
+      <c r="E487" s="2">
+        <v>-118.596958</v>
+      </c>
+      <c r="F487" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G487">
+        <v>71</v>
+      </c>
+      <c r="H487" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="488" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A488" s="3">
+        <v>127</v>
+      </c>
+      <c r="B488" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C488" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D488" s="2">
+        <v>34.416642000000003</v>
+      </c>
+      <c r="E488" s="2">
+        <v>-118.580106</v>
+      </c>
+      <c r="F488" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G488">
+        <v>67</v>
+      </c>
+      <c r="H488" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="489" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A489" s="3">
+        <v>127</v>
+      </c>
+      <c r="B489" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C489" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D489" s="2">
+        <v>34.416685000000001</v>
+      </c>
+      <c r="E489" s="2">
+        <v>-118.579657</v>
+      </c>
+      <c r="F489" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="G489">
+        <v>72</v>
+      </c>
+      <c r="H489" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="490" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A490" s="3">
+        <v>128</v>
+      </c>
+      <c r="B490" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C490" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D490" s="2">
+        <v>34.398218</v>
+      </c>
+      <c r="E490" s="2">
+        <v>-118.572524</v>
+      </c>
+      <c r="F490" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G490">
+        <v>66</v>
+      </c>
+      <c r="H490" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A491" s="3">
+        <v>128</v>
+      </c>
+      <c r="B491" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C491" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D491" s="2">
+        <v>34.398390999999997</v>
+      </c>
+      <c r="E491" s="2">
+        <v>-118.571989</v>
+      </c>
+      <c r="F491" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G491">
+        <v>73</v>
+      </c>
+      <c r="H491" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A492" s="3">
+        <v>129</v>
+      </c>
+      <c r="B492" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C492" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D492" s="2">
+        <v>34.381309000000002</v>
+      </c>
+      <c r="E492" s="2">
+        <v>-118.567223</v>
+      </c>
+      <c r="F492" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="G492">
+        <v>68</v>
+      </c>
+      <c r="H492" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A493" s="3">
+        <v>129</v>
+      </c>
+      <c r="B493" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C493" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D493" s="2">
+        <v>34.381591999999998</v>
+      </c>
+      <c r="E493" s="2">
+        <v>-118.566743</v>
+      </c>
+      <c r="F493" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G493">
+        <v>70</v>
+      </c>
+      <c r="H493" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A494" s="3">
+        <v>130</v>
+      </c>
+      <c r="B494" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C494" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D494" s="2">
+        <v>34.366025</v>
+      </c>
+      <c r="E494" s="2">
+        <v>-118.557295</v>
+      </c>
+      <c r="F494" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G494">
+        <v>68</v>
+      </c>
+      <c r="H494" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A495" s="3">
+        <v>130</v>
+      </c>
+      <c r="B495" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C495" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D495" s="2">
+        <v>34.366211999999997</v>
+      </c>
+      <c r="E495" s="2">
+        <v>-118.556828</v>
+      </c>
+      <c r="F495" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="G495">
+        <v>70</v>
+      </c>
+      <c r="H495" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A496" s="3">
+        <v>131</v>
+      </c>
+      <c r="B496" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C496" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D496" s="2">
+        <v>34.349165999999997</v>
+      </c>
+      <c r="E496" s="2">
+        <v>-118.54016900000001</v>
+      </c>
+      <c r="F496" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G496">
+        <v>68</v>
+      </c>
+      <c r="H496" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A497" s="3">
+        <v>132</v>
+      </c>
+      <c r="B497" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C497" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H497" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A498" s="3">
+        <v>131</v>
+      </c>
+      <c r="B498" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C498" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D498" s="2">
+        <v>34.349448000000002</v>
+      </c>
+      <c r="E498" s="2">
+        <v>-118.53963299999999</v>
+      </c>
+      <c r="F498" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G498">
+        <v>69</v>
+      </c>
+      <c r="H498" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A499" s="3">
+        <v>132</v>
+      </c>
+      <c r="B499" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C499" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H499" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A500" s="3">
+        <v>133</v>
+      </c>
+      <c r="B500" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C500" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D500" s="2">
+        <v>34.322656000000002</v>
+      </c>
+      <c r="E500" s="2">
+        <v>-118.499685</v>
+      </c>
+      <c r="F500" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G500">
+        <v>71</v>
+      </c>
+      <c r="H500" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A501" s="3">
+        <v>133</v>
+      </c>
+      <c r="B501" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C501" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D501" s="2">
+        <v>34.322941999999998</v>
+      </c>
+      <c r="E501" s="2">
+        <v>-118.499216</v>
+      </c>
+      <c r="F501" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G501">
+        <v>68</v>
+      </c>
+      <c r="H501" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A502" s="3">
+        <v>134</v>
+      </c>
+      <c r="B502" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C502" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D502" s="2">
+        <v>34.313791000000002</v>
+      </c>
+      <c r="E502" s="2">
+        <v>-118.48889</v>
+      </c>
+      <c r="F502" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="G502">
+        <v>63</v>
+      </c>
+      <c r="H502" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A503" s="3">
+        <v>134</v>
+      </c>
+      <c r="B503" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C503" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D503" s="2">
+        <v>34.313867999999999</v>
+      </c>
+      <c r="E503" s="2">
+        <v>-118.488527</v>
+      </c>
+      <c r="F503" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="G503">
+        <v>70</v>
+      </c>
+      <c r="H503" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A504" s="3">
+        <v>135</v>
+      </c>
+      <c r="B504" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C504" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D504" s="2">
+        <v>34.302182999999999</v>
+      </c>
+      <c r="E504" s="2">
+        <v>-118.47882799999999</v>
+      </c>
+      <c r="F504" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G504">
+        <v>71</v>
+      </c>
+      <c r="H504" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A505" s="3">
+        <v>135</v>
+      </c>
+      <c r="B505" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C505" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D505" s="2">
+        <v>34.302335999999997</v>
+      </c>
+      <c r="E505" s="2">
+        <v>-118.47851</v>
+      </c>
+      <c r="F505" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G505">
+        <v>69</v>
+      </c>
+      <c r="H505" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A506" s="3">
+        <v>144</v>
+      </c>
+      <c r="B506" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C506" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D506" s="2">
+        <v>34.285404</v>
+      </c>
+      <c r="E506" s="2">
+        <v>-118.46048500000001</v>
+      </c>
+      <c r="F506" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="G506">
+        <v>71</v>
+      </c>
+      <c r="H506" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A507" s="3">
+        <v>144</v>
+      </c>
+      <c r="B507" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C507" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D507" s="2">
+        <v>34.285578000000001</v>
+      </c>
+      <c r="E507" s="2">
+        <v>-118.460261</v>
+      </c>
+      <c r="F507" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G507">
+        <v>69</v>
+      </c>
+      <c r="H507" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A508" s="3">
+        <v>142</v>
+      </c>
+      <c r="B508" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C508" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D508" s="2">
+        <v>34.267550999999997</v>
+      </c>
+      <c r="E508" s="2">
+        <v>-118.44453300000001</v>
+      </c>
+      <c r="F508" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G508">
+        <v>73</v>
+      </c>
+      <c r="H508" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A509" s="3">
+        <v>142</v>
+      </c>
+      <c r="B509" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C509" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D509" s="2">
+        <v>34.267578999999998</v>
+      </c>
+      <c r="E509" s="2">
+        <v>-118.44413299999999</v>
+      </c>
+      <c r="F509" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G509">
+        <v>72</v>
+      </c>
+      <c r="H509" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A510" s="3">
+        <v>235</v>
+      </c>
+      <c r="B510" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C510" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D510" s="2">
+        <v>34.252446999999997</v>
+      </c>
+      <c r="E510" s="2">
+        <v>-118.43091099999999</v>
+      </c>
+      <c r="F510" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G510">
+        <v>70</v>
+      </c>
+      <c r="H510" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A511" s="3">
+        <v>235</v>
+      </c>
+      <c r="B511" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C511" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D511" s="2">
+        <v>34.248691999999998</v>
+      </c>
+      <c r="E511" s="2">
+        <v>-118.426293</v>
+      </c>
+      <c r="F511" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="G511">
+        <v>69</v>
+      </c>
+      <c r="H511" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A512" s="3">
+        <v>236</v>
+      </c>
+      <c r="B512" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C512" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D512" s="2"/>
+      <c r="E512" s="2"/>
+      <c r="F512" s="1"/>
+      <c r="H512" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A513" s="3">
+        <v>236</v>
+      </c>
+      <c r="B513" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C513" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D513" s="2">
+        <v>34.239215000000002</v>
+      </c>
+      <c r="E513" s="2">
+        <v>-118.416954</v>
+      </c>
+      <c r="F513" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G513">
+        <v>71</v>
+      </c>
+      <c r="H513" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A514" s="3">
+        <v>237</v>
+      </c>
+      <c r="B514" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C514" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D514" s="2">
+        <v>34.231746999999999</v>
+      </c>
+      <c r="E514" s="2">
+        <v>-118.40582999999999</v>
+      </c>
+      <c r="F514" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G514">
+        <v>70</v>
+      </c>
+      <c r="H514" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A515" s="3">
+        <v>237</v>
+      </c>
+      <c r="B515" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C515" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D515" s="2">
+        <v>34.231436000000002</v>
+      </c>
+      <c r="E515" s="2">
+        <v>-118.402399</v>
+      </c>
+      <c r="F515" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G515">
+        <v>70</v>
+      </c>
+      <c r="H515" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A516" s="3">
+        <v>238</v>
+      </c>
+      <c r="B516" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C516" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D516" s="2">
+        <v>34.226629000000003</v>
+      </c>
+      <c r="E516" s="2">
+        <v>-118.37799800000001</v>
+      </c>
+      <c r="F516" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G516">
+        <v>68</v>
+      </c>
+      <c r="H516" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A517" s="3">
+        <v>238</v>
+      </c>
+      <c r="B517" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C517" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D517" s="2">
+        <v>34.226914999999998</v>
+      </c>
+      <c r="E517" s="2">
+        <v>-118.37790800000001</v>
+      </c>
+      <c r="F517" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="G517">
+        <v>68</v>
+      </c>
+      <c r="H517" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A518" s="3">
+        <v>239</v>
+      </c>
+      <c r="B518" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C518" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H518" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A519" s="3">
+        <v>239</v>
+      </c>
+      <c r="B519" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C519" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D519" s="2">
+        <v>34.221127000000003</v>
+      </c>
+      <c r="E519" s="2">
+        <v>-118.35919800000001</v>
+      </c>
+      <c r="F519" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G519">
+        <v>70</v>
+      </c>
+      <c r="H519" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A520" s="3">
+        <v>240</v>
+      </c>
+      <c r="B520" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C520" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D520" s="2">
+        <v>34.203280999999997</v>
+      </c>
+      <c r="E520" s="2">
+        <v>-118.341182</v>
+      </c>
+      <c r="F520" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="G520">
+        <v>73</v>
+      </c>
+      <c r="H520" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A521" s="3">
+        <v>240</v>
+      </c>
+      <c r="B521" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C521" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D521" s="2">
+        <v>34.203507000000002</v>
+      </c>
+      <c r="E521" s="2">
+        <v>-118.340761</v>
+      </c>
+      <c r="F521" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G521">
+        <v>70</v>
+      </c>
+      <c r="H521" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A522" s="3">
+        <v>241</v>
+      </c>
+      <c r="B522" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C522" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D522" s="2">
+        <v>34.181851000000002</v>
+      </c>
+      <c r="E522" s="2">
+        <v>-118.31492900000001</v>
+      </c>
+      <c r="F522" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="G522">
+        <v>70</v>
+      </c>
+      <c r="H522" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A523" s="3">
+        <v>241</v>
+      </c>
+      <c r="B523" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C523" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D523" s="2">
+        <v>34.181786000000002</v>
+      </c>
+      <c r="E523" s="2">
+        <v>-118.314375</v>
+      </c>
+      <c r="F523" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G523">
+        <v>71</v>
+      </c>
+      <c r="H523" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A524" s="3">
+        <v>242</v>
+      </c>
+      <c r="B524" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C524" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D524" s="2">
+        <v>34.173495000000003</v>
+      </c>
+      <c r="E524" s="2">
+        <v>-118.30665399999999</v>
+      </c>
+      <c r="F524" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G524">
+        <v>69</v>
+      </c>
+      <c r="H524" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A525" s="3">
+        <v>242</v>
+      </c>
+      <c r="B525" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C525" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D525" s="2">
+        <v>34.173378</v>
+      </c>
+      <c r="E525" s="2">
+        <v>-118.306214</v>
+      </c>
+      <c r="F525" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="G525">
+        <v>65</v>
+      </c>
+      <c r="H525" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A526" s="3">
+        <v>243</v>
+      </c>
+      <c r="B526" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C526" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D526" s="2">
+        <v>34.158312000000002</v>
+      </c>
+      <c r="E526" s="2">
+        <v>-118.29170000000001</v>
+      </c>
+      <c r="F526" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="G526">
+        <v>71</v>
+      </c>
+      <c r="H526" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A527" s="3">
+        <v>243</v>
+      </c>
+      <c r="B527" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C527" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D527" s="2">
+        <v>34.158107000000001</v>
+      </c>
+      <c r="E527" s="2">
+        <v>-118.291191</v>
+      </c>
+      <c r="F527" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="G527">
+        <v>66</v>
+      </c>
+      <c r="H527" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A528" s="3">
+        <v>262</v>
+      </c>
+      <c r="B528" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C528" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D528" s="2">
+        <v>34.147053</v>
+      </c>
+      <c r="E528" s="2">
+        <v>-118.27934500000001</v>
+      </c>
+      <c r="F528" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G528">
+        <v>69</v>
+      </c>
+      <c r="H528" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="529" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A529" s="3">
+        <v>262</v>
+      </c>
+      <c r="B529" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C529" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D529" s="2">
+        <v>34.147038000000002</v>
+      </c>
+      <c r="E529" s="2">
+        <v>-118.278925</v>
+      </c>
+      <c r="F529" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="G529">
+        <v>66</v>
+      </c>
+      <c r="H529" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="530" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A530" s="3">
+        <v>263</v>
+      </c>
+      <c r="B530" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C530" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D530" s="2">
+        <v>34.128570000000003</v>
+      </c>
+      <c r="E530" s="2">
+        <v>-118.274084</v>
+      </c>
+      <c r="F530" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G530">
+        <v>69</v>
+      </c>
+      <c r="H530" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="531" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A531" s="3">
+        <v>263</v>
+      </c>
+      <c r="B531" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C531" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D531" s="2">
+        <v>34.128279999999997</v>
+      </c>
+      <c r="E531" s="2">
+        <v>-118.273579</v>
+      </c>
+      <c r="F531" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="G531">
+        <v>68</v>
+      </c>
+      <c r="H531" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="532" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A532" s="3">
+        <v>264</v>
+      </c>
+      <c r="B532" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C532" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D532" s="2">
+        <v>34.109602000000002</v>
+      </c>
+      <c r="E532" s="2">
+        <v>-118.26189599999999</v>
+      </c>
+      <c r="F532" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G532">
+        <v>64</v>
+      </c>
+      <c r="H532" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="533" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A533" s="3">
+        <v>264</v>
+      </c>
+      <c r="B533" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C533" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D533" s="2">
+        <v>34.109884999999998</v>
+      </c>
+      <c r="E533" s="2">
+        <v>-118.26170399999999</v>
+      </c>
+      <c r="F533" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G533">
+        <v>66</v>
+      </c>
+      <c r="H533" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="534" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A534" s="3">
+        <v>265</v>
+      </c>
+      <c r="B534" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C534" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D534" s="2">
+        <v>34.097011999999999</v>
+      </c>
+      <c r="E534" s="2">
+        <v>-118.24552300000001</v>
+      </c>
+      <c r="F534" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G534">
+        <v>64</v>
+      </c>
+      <c r="H534" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="535" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A535" s="3">
+        <v>265</v>
+      </c>
+      <c r="B535" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C535" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D535" s="2">
+        <v>34.097099</v>
+      </c>
+      <c r="E535" s="2">
+        <v>-118.24516</v>
+      </c>
+      <c r="F535" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G535">
+        <v>65</v>
+      </c>
+      <c r="H535" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="536" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A536" s="3">
+        <v>266</v>
+      </c>
+      <c r="B536" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C536" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D536" s="2">
+        <v>34.085574000000001</v>
+      </c>
+      <c r="E536" s="2">
+        <v>-118.23198499999999</v>
+      </c>
+      <c r="F536" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G536">
+        <v>65</v>
+      </c>
+      <c r="H536" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="537" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A537" s="3">
+        <v>266</v>
+      </c>
+      <c r="B537" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C537" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D537" s="2">
+        <v>34.085670999999998</v>
+      </c>
+      <c r="E537" s="2">
+        <v>-118.231697</v>
+      </c>
+      <c r="F537" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G537">
+        <v>68</v>
+      </c>
+      <c r="H537" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="538" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A538" s="3">
+        <v>267</v>
+      </c>
+      <c r="B538" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C538" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D538" s="2">
+        <v>34.070438000000003</v>
+      </c>
+      <c r="E538" s="2">
+        <v>-118.21813899999999</v>
+      </c>
+      <c r="F538" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="G538">
+        <v>62</v>
+      </c>
+      <c r="H538" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="539" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A539" s="3">
+        <v>267</v>
+      </c>
+      <c r="B539" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C539" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D539" s="2">
+        <v>34.070492000000002</v>
+      </c>
+      <c r="E539" s="2">
+        <v>-118.21789099999999</v>
+      </c>
+      <c r="F539" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="G539">
+        <v>65</v>
+      </c>
+      <c r="H539" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="540" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A540" s="3">
+        <v>268</v>
+      </c>
+      <c r="B540" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C540" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D540" s="2">
+        <v>34.055211999999997</v>
+      </c>
+      <c r="E540" s="2">
+        <v>-118.189082</v>
+      </c>
+      <c r="F540" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G540">
+        <v>69</v>
+      </c>
+      <c r="H540" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="541" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A541" s="3">
+        <v>268</v>
+      </c>
+      <c r="B541" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C541" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D541" s="2">
+        <v>34.055484999999997</v>
+      </c>
+      <c r="E541" s="2">
+        <v>-118.189044</v>
+      </c>
+      <c r="F541" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="G541">
+        <v>71</v>
+      </c>
+      <c r="H541" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="542" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A542" s="3">
+        <v>269</v>
+      </c>
+      <c r="B542" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C542" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D542" s="2">
+        <v>34.061225999999998</v>
+      </c>
+      <c r="E542" s="2">
+        <v>-118.16700899999999</v>
+      </c>
+      <c r="F542" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="G542">
+        <v>68</v>
+      </c>
+      <c r="H542" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="543" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A543" s="3">
+        <v>269</v>
+      </c>
+      <c r="B543" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C543" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D543" s="2">
+        <v>34.061452000000003</v>
+      </c>
+      <c r="E543" s="2">
+        <v>-118.166883</v>
+      </c>
+      <c r="F543" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G543">
+        <v>66</v>
+      </c>
+      <c r="H543" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="544" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A544" s="3">
+        <v>270</v>
+      </c>
+      <c r="B544" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C544" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D544" s="2">
+        <v>34.070551000000002</v>
+      </c>
+      <c r="E544" s="2">
+        <v>-118.14669499999999</v>
+      </c>
+      <c r="F544" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="G544">
+        <v>65</v>
+      </c>
+      <c r="H544" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="545" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A545" s="3">
+        <v>270</v>
+      </c>
+      <c r="B545" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C545" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D545" s="2">
+        <v>34.071012000000003</v>
+      </c>
+      <c r="E545" s="2">
+        <v>-118.14661700000001</v>
+      </c>
+      <c r="F545" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="G545">
+        <v>64</v>
+      </c>
+      <c r="H545" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="546" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A546" s="3">
+        <v>289</v>
+      </c>
+      <c r="B546" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C546" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D546" s="2">
+        <v>34.071413</v>
+      </c>
+      <c r="E546" s="2">
+        <v>-118.129822</v>
+      </c>
+      <c r="F546" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="G546">
+        <v>68</v>
+      </c>
+      <c r="H546" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="547" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A547" s="3">
+        <v>289</v>
+      </c>
+      <c r="B547" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C547" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D547" s="2">
+        <v>34.0717</v>
+      </c>
+      <c r="E547" s="2">
+        <v>-118.129846</v>
+      </c>
+      <c r="F547" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="G547">
+        <v>66</v>
+      </c>
+      <c r="H547" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="548" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A548" s="3">
+        <v>290</v>
+      </c>
+      <c r="B548" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C548" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D548" s="2">
+        <v>34.071809000000002</v>
+      </c>
+      <c r="E548" s="2">
+        <v>-118.09716400000001</v>
+      </c>
+      <c r="F548" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="G548">
+        <v>68</v>
+      </c>
+      <c r="H548" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="549" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A549" s="3">
+        <v>290</v>
+      </c>
+      <c r="B549" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C549" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D549" s="2">
+        <v>34.072152000000003</v>
+      </c>
+      <c r="E549" s="2">
+        <v>-118.097058</v>
+      </c>
+      <c r="F549" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="G549">
+        <v>67</v>
+      </c>
+      <c r="H549" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="550" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A550" s="3">
+        <v>291</v>
+      </c>
+      <c r="B550" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C550" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D550" s="2">
+        <v>34.072031000000003</v>
+      </c>
+      <c r="E550" s="2">
+        <v>-118.077432</v>
+      </c>
+      <c r="F550" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G550">
+        <v>69</v>
+      </c>
+      <c r="H550" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="551" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A551" s="3">
+        <v>292</v>
+      </c>
+      <c r="B551" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C551" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D551" s="2"/>
+      <c r="E551" s="2"/>
+      <c r="F551" s="1"/>
+      <c r="H551" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="552" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A552" s="3">
+        <v>291</v>
+      </c>
+      <c r="B552" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C552" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D552" s="2">
+        <v>34.072360000000003</v>
+      </c>
+      <c r="E552" s="2">
+        <v>-118.07747500000001</v>
+      </c>
+      <c r="F552" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G552">
+        <v>66</v>
+      </c>
+      <c r="H552" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="553" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A553" s="3">
+        <v>292</v>
+      </c>
+      <c r="B553" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C553" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D553" s="2">
+        <v>34.072535999999999</v>
+      </c>
+      <c r="E553" s="2">
+        <v>-118.066822</v>
+      </c>
+      <c r="F553" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="G553">
+        <v>68</v>
+      </c>
+      <c r="H553" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="554" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A554" s="3">
+        <v>293</v>
+      </c>
+      <c r="B554" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C554" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D554" s="2">
+        <v>34.067799999999998</v>
+      </c>
+      <c r="E554" s="2">
+        <v>-118.032729</v>
+      </c>
+      <c r="F554" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="G554">
+        <v>68</v>
+      </c>
+      <c r="H554" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="555" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A555" s="3">
+        <v>293</v>
+      </c>
+      <c r="B555" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C555" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D555" s="2">
+        <v>34.068095999999997</v>
+      </c>
+      <c r="E555" s="2">
+        <v>-118.03281200000001</v>
+      </c>
+      <c r="F555" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G555">
+        <v>70</v>
+      </c>
+      <c r="H555" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="556" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A556" s="3">
+        <v>294</v>
+      </c>
+      <c r="B556" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C556" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D556" s="2">
+        <v>34.064205000000001</v>
+      </c>
+      <c r="E556" s="2">
+        <v>-118.010711</v>
+      </c>
+      <c r="F556" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="G556">
+        <v>68</v>
+      </c>
+      <c r="H556" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="557" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A557" s="3">
+        <v>294</v>
+      </c>
+      <c r="B557" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C557" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D557" s="2">
+        <v>34.064452000000003</v>
+      </c>
+      <c r="E557" s="2">
+        <v>-118.01045999999999</v>
+      </c>
+      <c r="F557" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="G557">
+        <v>68</v>
+      </c>
+      <c r="H557" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="558" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A558" s="3">
+        <v>295</v>
+      </c>
+      <c r="B558" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C558" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D558" s="2">
+        <v>34.066215999999997</v>
+      </c>
+      <c r="E558" s="2">
+        <v>-117.990792</v>
+      </c>
+      <c r="F558" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="G558">
+        <v>65</v>
+      </c>
+      <c r="H558" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="559" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A559" s="3">
+        <v>295</v>
+      </c>
+      <c r="B559" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C559" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D559" s="2">
+        <v>34.066504000000002</v>
+      </c>
+      <c r="E559" s="2">
+        <v>-117.990825</v>
+      </c>
+      <c r="F559" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="G559">
+        <v>66</v>
+      </c>
+      <c r="H559" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="560" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A560" s="3">
+        <v>296</v>
+      </c>
+      <c r="B560" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C560" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D560" s="2">
+        <v>34.070264000000002</v>
+      </c>
+      <c r="E560" s="2">
+        <v>-117.960005</v>
+      </c>
+      <c r="F560" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G560">
+        <v>62</v>
+      </c>
+      <c r="H560" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="561" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A561" s="3">
+        <v>296</v>
+      </c>
+      <c r="B561" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C561" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D561" s="2">
+        <v>34.070528000000003</v>
+      </c>
+      <c r="E561" s="2">
+        <v>-117.95999399999999</v>
+      </c>
+      <c r="F561" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="G561">
+        <v>68</v>
+      </c>
+      <c r="H561" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="562" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A562" s="3">
+        <v>297</v>
+      </c>
+      <c r="B562" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C562" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D562" s="2">
+        <v>34.072271000000001</v>
+      </c>
+      <c r="E562" s="2">
+        <v>-117.938574</v>
+      </c>
+      <c r="F562" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="G562">
+        <v>71</v>
+      </c>
+      <c r="H562" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="563" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A563" s="3">
+        <v>297</v>
+      </c>
+      <c r="B563" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C563" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D563" s="2">
+        <v>34.072572999999998</v>
+      </c>
+      <c r="E563" s="2">
+        <v>-117.938512</v>
+      </c>
+      <c r="F563" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="G563">
+        <v>70</v>
+      </c>
+      <c r="H563" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="564" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A564" s="3">
+        <v>312</v>
+      </c>
+      <c r="B564" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C564" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D564" s="2">
+        <v>34.072066999999997</v>
+      </c>
+      <c r="E564" s="2">
+        <v>-117.915335</v>
+      </c>
+      <c r="F564" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="G564">
+        <v>70</v>
+      </c>
+      <c r="H564" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="565" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A565" s="3">
+        <v>312</v>
+      </c>
+      <c r="B565" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C565" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D565" s="2">
+        <v>34.072378999999998</v>
+      </c>
+      <c r="E565" s="2">
+        <v>-117.915308</v>
+      </c>
+      <c r="F565" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G565">
+        <v>71</v>
+      </c>
+      <c r="H565" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="566" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A566" s="3">
+        <v>311</v>
+      </c>
+      <c r="B566" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C566" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D566" s="2">
+        <v>34.071919000000001</v>
+      </c>
+      <c r="E566" s="2">
+        <v>-117.899631</v>
+      </c>
+      <c r="F566" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="G566">
+        <v>70</v>
+      </c>
+      <c r="H566" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="567" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A567" s="3">
+        <v>311</v>
+      </c>
+      <c r="B567" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C567" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D567" s="2">
+        <v>34.072226999999998</v>
+      </c>
+      <c r="E567" s="2">
+        <v>-117.899615</v>
+      </c>
+      <c r="F567" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="G567">
+        <v>70</v>
+      </c>
+      <c r="H567" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix led locations and add to source code
</commit_message>
<xml_diff>
--- a/led_locations.xlsx
+++ b/led_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDFEB85-CD9B-45AC-8127-EC9F5B474752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ACA3A6-C04A-428F-940F-EFEA5C39B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="554">
   <si>
     <t>LED Number</t>
   </si>
@@ -2035,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H653"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="D659" sqref="D659"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,6 +2165,18 @@
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>-2</v>
+      </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
@@ -2205,6 +2217,18 @@
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>-2</v>
+      </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
@@ -2245,6 +2269,18 @@
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>-4</v>
+      </c>
       <c r="H9" t="s">
         <v>14</v>
       </c>
@@ -2285,6 +2321,18 @@
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>-4</v>
+      </c>
       <c r="H11" t="s">
         <v>14</v>
       </c>
@@ -3001,6 +3049,18 @@
       <c r="C39" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>-19</v>
+      </c>
       <c r="H39" t="s">
         <v>14</v>
       </c>
@@ -3067,6 +3127,18 @@
       <c r="C42" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>-20</v>
+      </c>
       <c r="H42" t="s">
         <v>14</v>
       </c>
@@ -3107,7 +3179,18 @@
       <c r="C44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>-21</v>
+      </c>
       <c r="H44" t="s">
         <v>14</v>
       </c>
@@ -3278,9 +3361,18 @@
       <c r="C51" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="1"/>
+      <c r="D51" s="2">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>-26</v>
+      </c>
       <c r="H51" t="s">
         <v>14</v>
       </c>
@@ -3321,6 +3413,18 @@
       <c r="C53" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D53" s="2">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>-25</v>
+      </c>
       <c r="H53" t="s">
         <v>14</v>
       </c>
@@ -3335,6 +3439,18 @@
       <c r="C54" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>-25</v>
+      </c>
       <c r="H54" t="s">
         <v>14</v>
       </c>
@@ -3349,6 +3465,18 @@
       <c r="C55" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D55" s="2">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>-25</v>
+      </c>
       <c r="H55" t="s">
         <v>14</v>
       </c>
@@ -3363,6 +3491,18 @@
       <c r="C56" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D56" s="2">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>-25</v>
+      </c>
       <c r="H56" t="s">
         <v>14</v>
       </c>
@@ -3377,6 +3517,18 @@
       <c r="C57" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>-25</v>
+      </c>
       <c r="H57" t="s">
         <v>14</v>
       </c>
@@ -3391,6 +3543,18 @@
       <c r="C58" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D58" s="2">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>-25</v>
+      </c>
       <c r="H58" t="s">
         <v>14</v>
       </c>
@@ -3405,6 +3569,18 @@
       <c r="C59" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D59" s="2">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>-25</v>
+      </c>
       <c r="H59" t="s">
         <v>14</v>
       </c>
@@ -3445,6 +3621,18 @@
       <c r="C61" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+      <c r="F61" s="3">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>-27</v>
+      </c>
       <c r="H61" t="s">
         <v>14</v>
       </c>
@@ -3459,6 +3647,18 @@
       <c r="C62" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>-27</v>
+      </c>
       <c r="H62" t="s">
         <v>14</v>
       </c>
@@ -3473,6 +3673,18 @@
       <c r="C63" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D63" s="2">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>-27</v>
+      </c>
       <c r="H63" t="s">
         <v>14</v>
       </c>
@@ -3487,6 +3699,18 @@
       <c r="C64" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D64" s="2">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>-27</v>
+      </c>
       <c r="H64" t="s">
         <v>14</v>
       </c>
@@ -3501,6 +3725,18 @@
       <c r="C65" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D65" s="2">
+        <v>0</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>-27</v>
+      </c>
       <c r="H65" t="s">
         <v>14</v>
       </c>
@@ -3515,6 +3751,18 @@
       <c r="C66" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D66" s="2">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0</v>
+      </c>
+      <c r="F66" s="3">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>-27</v>
+      </c>
       <c r="H66" t="s">
         <v>14</v>
       </c>
@@ -3607,6 +3855,18 @@
       <c r="C70" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D70" s="2">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0</v>
+      </c>
+      <c r="F70" s="3">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>-34</v>
+      </c>
       <c r="H70" t="s">
         <v>14</v>
       </c>
@@ -3751,6 +4011,18 @@
       <c r="C76" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D76" s="2">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0</v>
+      </c>
+      <c r="F76" s="3">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>-37</v>
+      </c>
       <c r="H76" t="s">
         <v>14</v>
       </c>
@@ -4147,7 +4419,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B92" s="3">
         <v>101</v>
@@ -4173,7 +4445,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B93" s="3">
         <v>101</v>
@@ -4207,6 +4479,18 @@
       <c r="C94" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D94" s="2">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2">
+        <v>0</v>
+      </c>
+      <c r="F94" s="3">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>-73</v>
+      </c>
       <c r="H94" t="s">
         <v>14</v>
       </c>
@@ -4325,6 +4609,18 @@
       <c r="C99" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D99" s="2">
+        <v>0</v>
+      </c>
+      <c r="E99" s="2">
+        <v>0</v>
+      </c>
+      <c r="F99" s="3">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>-76</v>
+      </c>
       <c r="H99" t="s">
         <v>14</v>
       </c>
@@ -4365,6 +4661,18 @@
       <c r="C101" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D101" s="2">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2">
+        <v>0</v>
+      </c>
+      <c r="F101" s="3">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>-76</v>
+      </c>
       <c r="H101" t="s">
         <v>14</v>
       </c>
@@ -4587,6 +4895,18 @@
       <c r="C110" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D110" s="2">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2">
+        <v>0</v>
+      </c>
+      <c r="F110" s="3">
+        <v>0</v>
+      </c>
+      <c r="G110">
+        <v>-81</v>
+      </c>
       <c r="H110" t="s">
         <v>14</v>
       </c>
@@ -4965,6 +5285,18 @@
       <c r="C125" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D125" s="2">
+        <v>0</v>
+      </c>
+      <c r="E125" s="2">
+        <v>0</v>
+      </c>
+      <c r="F125" s="3">
+        <v>0</v>
+      </c>
+      <c r="G125">
+        <v>-107</v>
+      </c>
       <c r="H125" t="s">
         <v>14</v>
       </c>
@@ -5005,6 +5337,18 @@
       <c r="C127" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D127" s="2">
+        <v>0</v>
+      </c>
+      <c r="E127" s="2">
+        <v>0</v>
+      </c>
+      <c r="F127" s="3">
+        <v>0</v>
+      </c>
+      <c r="G127">
+        <v>-107</v>
+      </c>
       <c r="H127" t="s">
         <v>14</v>
       </c>
@@ -5123,6 +5467,18 @@
       <c r="C132" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D132" s="2">
+        <v>0</v>
+      </c>
+      <c r="E132" s="2">
+        <v>0</v>
+      </c>
+      <c r="F132" s="3">
+        <v>0</v>
+      </c>
+      <c r="G132">
+        <v>-146</v>
+      </c>
       <c r="H132" t="s">
         <v>14</v>
       </c>
@@ -5137,6 +5493,18 @@
       <c r="C133" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D133" s="2">
+        <v>0</v>
+      </c>
+      <c r="E133" s="2">
+        <v>0</v>
+      </c>
+      <c r="F133" s="3">
+        <v>0</v>
+      </c>
+      <c r="G133">
+        <v>-146</v>
+      </c>
       <c r="H133" t="s">
         <v>14</v>
       </c>
@@ -5151,6 +5519,18 @@
       <c r="C134" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D134" s="2">
+        <v>0</v>
+      </c>
+      <c r="E134" s="2">
+        <v>0</v>
+      </c>
+      <c r="F134" s="3">
+        <v>0</v>
+      </c>
+      <c r="G134">
+        <v>-146</v>
+      </c>
       <c r="H134" t="s">
         <v>14</v>
       </c>
@@ -5815,6 +6195,18 @@
       <c r="C160" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D160" s="2">
+        <v>0</v>
+      </c>
+      <c r="E160" s="2">
+        <v>0</v>
+      </c>
+      <c r="F160" s="3">
+        <v>0</v>
+      </c>
+      <c r="G160">
+        <v>-250</v>
+      </c>
       <c r="H160" t="s">
         <v>14</v>
       </c>
@@ -5829,6 +6221,21 @@
       <c r="C161" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D161" s="2">
+        <v>0</v>
+      </c>
+      <c r="E161" s="2">
+        <v>0</v>
+      </c>
+      <c r="F161" s="3">
+        <v>0</v>
+      </c>
+      <c r="G161">
+        <v>-250</v>
+      </c>
+      <c r="H161" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
@@ -7478,6 +7885,18 @@
       <c r="C225" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D225" s="2">
+        <v>0</v>
+      </c>
+      <c r="E225" s="2">
+        <v>0</v>
+      </c>
+      <c r="F225" s="3">
+        <v>0</v>
+      </c>
+      <c r="G225">
+        <v>-61</v>
+      </c>
       <c r="H225" t="s">
         <v>14</v>
       </c>
@@ -7492,6 +7911,18 @@
       <c r="C226" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D226" s="2">
+        <v>0</v>
+      </c>
+      <c r="E226" s="2">
+        <v>0</v>
+      </c>
+      <c r="F226" s="3">
+        <v>0</v>
+      </c>
+      <c r="G226">
+        <v>-61</v>
+      </c>
       <c r="H226" t="s">
         <v>14</v>
       </c>
@@ -7506,6 +7937,18 @@
       <c r="C227" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D227" s="2">
+        <v>0</v>
+      </c>
+      <c r="E227" s="2">
+        <v>0</v>
+      </c>
+      <c r="F227" s="3">
+        <v>0</v>
+      </c>
+      <c r="G227">
+        <v>-61</v>
+      </c>
       <c r="H227" t="s">
         <v>14</v>
       </c>
@@ -7520,6 +7963,18 @@
       <c r="C228" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D228" s="2">
+        <v>0</v>
+      </c>
+      <c r="E228" s="2">
+        <v>0</v>
+      </c>
+      <c r="F228" s="3">
+        <v>0</v>
+      </c>
+      <c r="G228">
+        <v>-61</v>
+      </c>
       <c r="H228" t="s">
         <v>14</v>
       </c>
@@ -7534,6 +7989,18 @@
       <c r="C229" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D229" s="2">
+        <v>0</v>
+      </c>
+      <c r="E229" s="2">
+        <v>0</v>
+      </c>
+      <c r="F229" s="3">
+        <v>0</v>
+      </c>
+      <c r="G229">
+        <v>-61</v>
+      </c>
       <c r="H229" t="s">
         <v>14</v>
       </c>
@@ -7574,6 +8041,21 @@
       <c r="C231" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D231" s="2">
+        <v>0</v>
+      </c>
+      <c r="E231" s="2">
+        <v>0</v>
+      </c>
+      <c r="F231" s="3">
+        <v>0</v>
+      </c>
+      <c r="G231">
+        <v>-61</v>
+      </c>
+      <c r="H231" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
@@ -7585,6 +8067,21 @@
       <c r="C232" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D232" s="2">
+        <v>0</v>
+      </c>
+      <c r="E232" s="2">
+        <v>0</v>
+      </c>
+      <c r="F232" s="3">
+        <v>0</v>
+      </c>
+      <c r="G232">
+        <v>-61</v>
+      </c>
+      <c r="H232" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
@@ -7596,6 +8093,21 @@
       <c r="C233" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D233" s="2">
+        <v>0</v>
+      </c>
+      <c r="E233" s="2">
+        <v>0</v>
+      </c>
+      <c r="F233" s="3">
+        <v>0</v>
+      </c>
+      <c r="G233">
+        <v>-61</v>
+      </c>
+      <c r="H233" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
@@ -7607,6 +8119,21 @@
       <c r="C234" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D234" s="2">
+        <v>0</v>
+      </c>
+      <c r="E234" s="2">
+        <v>0</v>
+      </c>
+      <c r="F234" s="3">
+        <v>0</v>
+      </c>
+      <c r="G234">
+        <v>-61</v>
+      </c>
+      <c r="H234" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
@@ -7618,6 +8145,21 @@
       <c r="C235" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D235" s="2">
+        <v>0</v>
+      </c>
+      <c r="E235" s="2">
+        <v>0</v>
+      </c>
+      <c r="F235" s="3">
+        <v>0</v>
+      </c>
+      <c r="G235">
+        <v>-61</v>
+      </c>
+      <c r="H235" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
@@ -7655,6 +8197,18 @@
       <c r="C237" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D237" s="2">
+        <v>0</v>
+      </c>
+      <c r="E237" s="2">
+        <v>0</v>
+      </c>
+      <c r="F237" s="3">
+        <v>0</v>
+      </c>
+      <c r="G237">
+        <v>-85</v>
+      </c>
       <c r="H237" t="s">
         <v>14</v>
       </c>
@@ -7695,6 +8249,18 @@
       <c r="C239" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D239" s="2">
+        <v>0</v>
+      </c>
+      <c r="E239" s="2">
+        <v>0</v>
+      </c>
+      <c r="F239" s="3">
+        <v>0</v>
+      </c>
+      <c r="G239">
+        <v>-85</v>
+      </c>
       <c r="H239" t="s">
         <v>14</v>
       </c>
@@ -7735,6 +8301,18 @@
       <c r="C241" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D241" s="2">
+        <v>0</v>
+      </c>
+      <c r="E241" s="2">
+        <v>0</v>
+      </c>
+      <c r="F241" s="3">
+        <v>0</v>
+      </c>
+      <c r="G241">
+        <v>-87</v>
+      </c>
       <c r="H241" t="s">
         <v>14</v>
       </c>
@@ -7775,6 +8353,18 @@
       <c r="C243" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D243" s="2">
+        <v>0</v>
+      </c>
+      <c r="E243" s="2">
+        <v>0</v>
+      </c>
+      <c r="F243" s="3">
+        <v>0</v>
+      </c>
+      <c r="G243">
+        <v>-87</v>
+      </c>
       <c r="H243" t="s">
         <v>14</v>
       </c>
@@ -7815,6 +8405,18 @@
       <c r="C245" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D245" s="2">
+        <v>0</v>
+      </c>
+      <c r="E245" s="2">
+        <v>0</v>
+      </c>
+      <c r="F245" s="3">
+        <v>0</v>
+      </c>
+      <c r="G245">
+        <v>-89</v>
+      </c>
       <c r="H245" t="s">
         <v>14</v>
       </c>
@@ -7829,6 +8431,18 @@
       <c r="C246" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D246" s="2">
+        <v>0</v>
+      </c>
+      <c r="E246" s="2">
+        <v>0</v>
+      </c>
+      <c r="F246" s="3">
+        <v>0</v>
+      </c>
+      <c r="G246">
+        <v>-89</v>
+      </c>
       <c r="H246" t="s">
         <v>14</v>
       </c>
@@ -7843,6 +8457,18 @@
       <c r="C247" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D247" s="2">
+        <v>0</v>
+      </c>
+      <c r="E247" s="2">
+        <v>0</v>
+      </c>
+      <c r="F247" s="3">
+        <v>0</v>
+      </c>
+      <c r="G247">
+        <v>-89</v>
+      </c>
       <c r="H247" t="s">
         <v>14</v>
       </c>
@@ -7883,6 +8509,21 @@
       <c r="C249" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D249" s="2">
+        <v>0</v>
+      </c>
+      <c r="E249" s="2">
+        <v>0</v>
+      </c>
+      <c r="F249" s="3">
+        <v>0</v>
+      </c>
+      <c r="G249">
+        <v>-88</v>
+      </c>
+      <c r="H249" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="3">
@@ -7894,6 +8535,21 @@
       <c r="C250" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D250" s="2">
+        <v>0</v>
+      </c>
+      <c r="E250" s="2">
+        <v>0</v>
+      </c>
+      <c r="F250" s="3">
+        <v>0</v>
+      </c>
+      <c r="G250">
+        <v>-88</v>
+      </c>
+      <c r="H250" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="3">
@@ -7905,6 +8561,21 @@
       <c r="C251" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D251" s="2">
+        <v>0</v>
+      </c>
+      <c r="E251" s="2">
+        <v>0</v>
+      </c>
+      <c r="F251" s="3">
+        <v>0</v>
+      </c>
+      <c r="G251">
+        <v>-88</v>
+      </c>
+      <c r="H251" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
@@ -7994,6 +8665,18 @@
       <c r="C255" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D255" s="2">
+        <v>0</v>
+      </c>
+      <c r="E255" s="2">
+        <v>0</v>
+      </c>
+      <c r="F255" s="3">
+        <v>0</v>
+      </c>
+      <c r="G255">
+        <v>-112</v>
+      </c>
       <c r="H255" t="s">
         <v>14</v>
       </c>
@@ -8034,6 +8717,18 @@
       <c r="C257" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D257" s="2">
+        <v>0</v>
+      </c>
+      <c r="E257" s="2">
+        <v>0</v>
+      </c>
+      <c r="F257" s="3">
+        <v>0</v>
+      </c>
+      <c r="G257">
+        <v>-112</v>
+      </c>
       <c r="H257" t="s">
         <v>14</v>
       </c>
@@ -8074,6 +8769,18 @@
       <c r="C259" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D259" s="2">
+        <v>0</v>
+      </c>
+      <c r="E259" s="2">
+        <v>0</v>
+      </c>
+      <c r="F259" s="3">
+        <v>0</v>
+      </c>
+      <c r="G259">
+        <v>-114</v>
+      </c>
       <c r="H259" t="s">
         <v>14</v>
       </c>
@@ -8114,6 +8821,18 @@
       <c r="C261" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D261" s="2">
+        <v>0</v>
+      </c>
+      <c r="E261" s="2">
+        <v>0</v>
+      </c>
+      <c r="F261" s="3">
+        <v>0</v>
+      </c>
+      <c r="G261">
+        <v>-114</v>
+      </c>
       <c r="H261" t="s">
         <v>14</v>
       </c>
@@ -8154,6 +8873,18 @@
       <c r="C263" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D263" s="2">
+        <v>0</v>
+      </c>
+      <c r="E263" s="2">
+        <v>0</v>
+      </c>
+      <c r="F263" s="3">
+        <v>0</v>
+      </c>
+      <c r="G263">
+        <v>-116</v>
+      </c>
       <c r="H263" t="s">
         <v>14</v>
       </c>
@@ -8168,6 +8899,18 @@
       <c r="C264" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D264" s="2">
+        <v>0</v>
+      </c>
+      <c r="E264" s="2">
+        <v>0</v>
+      </c>
+      <c r="F264" s="3">
+        <v>0</v>
+      </c>
+      <c r="G264">
+        <v>-116</v>
+      </c>
       <c r="H264" t="s">
         <v>14</v>
       </c>
@@ -8208,6 +8951,18 @@
       <c r="C266" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D266" s="2">
+        <v>0</v>
+      </c>
+      <c r="E266" s="2">
+        <v>0</v>
+      </c>
+      <c r="F266" s="3">
+        <v>0</v>
+      </c>
+      <c r="G266">
+        <v>-116</v>
+      </c>
       <c r="H266" t="s">
         <v>14</v>
       </c>
@@ -8222,6 +8977,18 @@
       <c r="C267" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D267" s="2">
+        <v>0</v>
+      </c>
+      <c r="E267" s="2">
+        <v>0</v>
+      </c>
+      <c r="F267" s="3">
+        <v>0</v>
+      </c>
+      <c r="G267">
+        <v>-116</v>
+      </c>
       <c r="H267" t="s">
         <v>14</v>
       </c>
@@ -8262,6 +9029,18 @@
       <c r="C269" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D269" s="2">
+        <v>0</v>
+      </c>
+      <c r="E269" s="2">
+        <v>0</v>
+      </c>
+      <c r="F269" s="3">
+        <v>0</v>
+      </c>
+      <c r="G269">
+        <v>-155</v>
+      </c>
       <c r="H269" t="s">
         <v>14</v>
       </c>
@@ -8276,6 +9055,18 @@
       <c r="C270" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D270" s="2">
+        <v>0</v>
+      </c>
+      <c r="E270" s="2">
+        <v>0</v>
+      </c>
+      <c r="F270" s="3">
+        <v>0</v>
+      </c>
+      <c r="G270">
+        <v>-155</v>
+      </c>
       <c r="H270" t="s">
         <v>14</v>
       </c>
@@ -8290,6 +9081,18 @@
       <c r="C271" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D271" s="2">
+        <v>0</v>
+      </c>
+      <c r="E271" s="2">
+        <v>0</v>
+      </c>
+      <c r="F271" s="3">
+        <v>0</v>
+      </c>
+      <c r="G271">
+        <v>-155</v>
+      </c>
       <c r="H271" t="s">
         <v>14</v>
       </c>
@@ -8330,6 +9133,18 @@
       <c r="C273" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D273" s="2">
+        <v>0</v>
+      </c>
+      <c r="E273" s="2">
+        <v>0</v>
+      </c>
+      <c r="F273" s="3">
+        <v>0</v>
+      </c>
+      <c r="G273">
+        <v>-155</v>
+      </c>
       <c r="H273" t="s">
         <v>14</v>
       </c>
@@ -8344,6 +9159,18 @@
       <c r="C274" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D274" s="2">
+        <v>0</v>
+      </c>
+      <c r="E274" s="2">
+        <v>0</v>
+      </c>
+      <c r="F274" s="3">
+        <v>0</v>
+      </c>
+      <c r="G274">
+        <v>-155</v>
+      </c>
       <c r="H274" t="s">
         <v>14</v>
       </c>
@@ -8722,6 +9549,18 @@
       <c r="C289" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D289" s="2">
+        <v>0</v>
+      </c>
+      <c r="E289" s="2">
+        <v>0</v>
+      </c>
+      <c r="F289" s="3">
+        <v>0</v>
+      </c>
+      <c r="G289">
+        <v>-192</v>
+      </c>
       <c r="H289" t="s">
         <v>14</v>
       </c>
@@ -9490,6 +10329,18 @@
       <c r="C319" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D319" s="2">
+        <v>0</v>
+      </c>
+      <c r="E319" s="2">
+        <v>0</v>
+      </c>
+      <c r="F319" s="3">
+        <v>0</v>
+      </c>
+      <c r="G319">
+        <v>-207</v>
+      </c>
       <c r="H319" t="s">
         <v>14</v>
       </c>
@@ -9530,6 +10381,18 @@
       <c r="C321" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D321" s="2">
+        <v>0</v>
+      </c>
+      <c r="E321" s="2">
+        <v>0</v>
+      </c>
+      <c r="F321" s="3">
+        <v>0</v>
+      </c>
+      <c r="G321">
+        <v>-207</v>
+      </c>
       <c r="H321" t="s">
         <v>14</v>
       </c>
@@ -9882,6 +10745,18 @@
       <c r="C335" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D335" s="2">
+        <v>0</v>
+      </c>
+      <c r="E335" s="2">
+        <v>0</v>
+      </c>
+      <c r="F335" s="3">
+        <v>0</v>
+      </c>
+      <c r="G335">
+        <v>-233</v>
+      </c>
       <c r="H335" t="s">
         <v>14</v>
       </c>
@@ -9922,6 +10797,18 @@
       <c r="C337" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D337" s="2">
+        <v>0</v>
+      </c>
+      <c r="E337" s="2">
+        <v>0</v>
+      </c>
+      <c r="F337" s="3">
+        <v>0</v>
+      </c>
+      <c r="G337">
+        <v>-233</v>
+      </c>
       <c r="H337" t="s">
         <v>14</v>
       </c>
@@ -9962,6 +10849,18 @@
       <c r="C339" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D339" s="2">
+        <v>0</v>
+      </c>
+      <c r="E339" s="2">
+        <v>0</v>
+      </c>
+      <c r="F339" s="3">
+        <v>0</v>
+      </c>
+      <c r="G339">
+        <v>-329</v>
+      </c>
       <c r="H339" t="s">
         <v>14</v>
       </c>
@@ -10002,6 +10901,18 @@
       <c r="C341" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D341" s="2">
+        <v>0</v>
+      </c>
+      <c r="E341" s="2">
+        <v>0</v>
+      </c>
+      <c r="F341" s="3">
+        <v>0</v>
+      </c>
+      <c r="G341">
+        <v>-329</v>
+      </c>
       <c r="H341" t="s">
         <v>14</v>
       </c>
@@ -10458,9 +11369,18 @@
       <c r="C359" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D359" s="2"/>
-      <c r="E359" s="2"/>
-      <c r="F359" s="1"/>
+      <c r="D359" s="2">
+        <v>0</v>
+      </c>
+      <c r="E359" s="2">
+        <v>0</v>
+      </c>
+      <c r="F359" s="3">
+        <v>0</v>
+      </c>
+      <c r="G359">
+        <v>-54</v>
+      </c>
       <c r="H359" t="s">
         <v>14</v>
       </c>
@@ -10501,6 +11421,18 @@
       <c r="C361" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D361" s="2">
+        <v>0</v>
+      </c>
+      <c r="E361" s="2">
+        <v>0</v>
+      </c>
+      <c r="F361" s="3">
+        <v>0</v>
+      </c>
+      <c r="G361">
+        <v>-54</v>
+      </c>
       <c r="H361" t="s">
         <v>14</v>
       </c>
@@ -10801,9 +11733,18 @@
       <c r="C373" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D373" s="2"/>
-      <c r="E373" s="2"/>
-      <c r="F373" s="1"/>
+      <c r="D373" s="2">
+        <v>0</v>
+      </c>
+      <c r="E373" s="2">
+        <v>0</v>
+      </c>
+      <c r="F373" s="3">
+        <v>0</v>
+      </c>
+      <c r="G373">
+        <v>-70</v>
+      </c>
       <c r="H373" t="s">
         <v>14</v>
       </c>
@@ -10818,9 +11759,18 @@
       <c r="C374" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D374" s="2"/>
-      <c r="E374" s="2"/>
-      <c r="F374" s="1"/>
+      <c r="D374" s="2">
+        <v>0</v>
+      </c>
+      <c r="E374" s="2">
+        <v>0</v>
+      </c>
+      <c r="F374" s="3">
+        <v>0</v>
+      </c>
+      <c r="G374">
+        <v>-70</v>
+      </c>
       <c r="H374" t="s">
         <v>14</v>
       </c>
@@ -10861,6 +11811,18 @@
       <c r="C376" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D376" s="2">
+        <v>0</v>
+      </c>
+      <c r="E376" s="2">
+        <v>0</v>
+      </c>
+      <c r="F376" s="3">
+        <v>0</v>
+      </c>
+      <c r="G376">
+        <v>-70</v>
+      </c>
       <c r="H376" t="s">
         <v>14</v>
       </c>
@@ -11187,6 +12149,18 @@
       <c r="C389" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D389" s="2">
+        <v>0</v>
+      </c>
+      <c r="E389" s="2">
+        <v>0</v>
+      </c>
+      <c r="F389" s="3">
+        <v>0</v>
+      </c>
+      <c r="G389">
+        <v>-96</v>
+      </c>
       <c r="H389" t="s">
         <v>14</v>
       </c>
@@ -11227,6 +12201,18 @@
       <c r="C391" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D391" s="2">
+        <v>0</v>
+      </c>
+      <c r="E391" s="2">
+        <v>0</v>
+      </c>
+      <c r="F391" s="3">
+        <v>0</v>
+      </c>
+      <c r="G391">
+        <v>-96</v>
+      </c>
       <c r="H391" t="s">
         <v>14</v>
       </c>
@@ -11475,6 +12461,18 @@
       <c r="C401" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D401" s="2">
+        <v>0</v>
+      </c>
+      <c r="E401" s="2">
+        <v>0</v>
+      </c>
+      <c r="F401" s="3">
+        <v>0</v>
+      </c>
+      <c r="G401">
+        <v>-138</v>
+      </c>
       <c r="H401" t="s">
         <v>14</v>
       </c>
@@ -11931,6 +12929,18 @@
       <c r="C419" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D419" s="2">
+        <v>0</v>
+      </c>
+      <c r="E419" s="2">
+        <v>0</v>
+      </c>
+      <c r="F419" s="3">
+        <v>0</v>
+      </c>
+      <c r="G419">
+        <v>-166</v>
+      </c>
       <c r="H419" t="s">
         <v>14</v>
       </c>
@@ -12075,6 +13085,18 @@
       <c r="C425" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D425" s="2">
+        <v>0</v>
+      </c>
+      <c r="E425" s="2">
+        <v>0</v>
+      </c>
+      <c r="F425" s="3">
+        <v>0</v>
+      </c>
+      <c r="G425">
+        <v>-169</v>
+      </c>
       <c r="H425" t="s">
         <v>14</v>
       </c>
@@ -12141,6 +13163,18 @@
       <c r="C428" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D428" s="2">
+        <v>0</v>
+      </c>
+      <c r="E428" s="2">
+        <v>0</v>
+      </c>
+      <c r="F428" s="3">
+        <v>0</v>
+      </c>
+      <c r="G428">
+        <v>-170</v>
+      </c>
       <c r="H428" t="s">
         <v>14</v>
       </c>
@@ -12155,6 +13189,18 @@
       <c r="C429" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D429" s="2">
+        <v>0</v>
+      </c>
+      <c r="E429" s="2">
+        <v>0</v>
+      </c>
+      <c r="F429" s="3">
+        <v>0</v>
+      </c>
+      <c r="G429">
+        <v>-170</v>
+      </c>
       <c r="H429" t="s">
         <v>14</v>
       </c>
@@ -12169,6 +13215,18 @@
       <c r="C430" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D430" s="2">
+        <v>0</v>
+      </c>
+      <c r="E430" s="2">
+        <v>0</v>
+      </c>
+      <c r="F430" s="3">
+        <v>0</v>
+      </c>
+      <c r="G430">
+        <v>-170</v>
+      </c>
       <c r="H430" t="s">
         <v>14</v>
       </c>
@@ -12209,6 +13267,18 @@
       <c r="C432" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D432" s="2">
+        <v>0</v>
+      </c>
+      <c r="E432" s="2">
+        <v>0</v>
+      </c>
+      <c r="F432" s="3">
+        <v>0</v>
+      </c>
+      <c r="G432">
+        <v>-171</v>
+      </c>
       <c r="H432" t="s">
         <v>14</v>
       </c>
@@ -12405,6 +13475,18 @@
       <c r="C440" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D440" s="2">
+        <v>0</v>
+      </c>
+      <c r="E440" s="2">
+        <v>0</v>
+      </c>
+      <c r="F440" s="3">
+        <v>0</v>
+      </c>
+      <c r="G440">
+        <v>-257</v>
+      </c>
       <c r="H440" t="s">
         <v>14</v>
       </c>
@@ -13251,6 +14333,18 @@
       <c r="C473" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D473" s="2">
+        <v>0</v>
+      </c>
+      <c r="E473" s="2">
+        <v>0</v>
+      </c>
+      <c r="F473" s="3">
+        <v>0</v>
+      </c>
+      <c r="G473">
+        <v>-118</v>
+      </c>
       <c r="H473" t="s">
         <v>14</v>
       </c>
@@ -13265,6 +14359,18 @@
       <c r="C474" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D474" s="2">
+        <v>0</v>
+      </c>
+      <c r="E474" s="2">
+        <v>0</v>
+      </c>
+      <c r="F474" s="3">
+        <v>0</v>
+      </c>
+      <c r="G474">
+        <v>-118</v>
+      </c>
       <c r="H474" t="s">
         <v>14</v>
       </c>
@@ -13279,6 +14385,18 @@
       <c r="C475" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D475" s="2">
+        <v>0</v>
+      </c>
+      <c r="E475" s="2">
+        <v>0</v>
+      </c>
+      <c r="F475" s="3">
+        <v>0</v>
+      </c>
+      <c r="G475">
+        <v>-118</v>
+      </c>
       <c r="H475" t="s">
         <v>14</v>
       </c>
@@ -13319,6 +14437,18 @@
       <c r="C477" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D477" s="2">
+        <v>0</v>
+      </c>
+      <c r="E477" s="2">
+        <v>0</v>
+      </c>
+      <c r="F477" s="3">
+        <v>0</v>
+      </c>
+      <c r="G477">
+        <v>-118</v>
+      </c>
       <c r="H477" t="s">
         <v>14</v>
       </c>
@@ -13333,6 +14463,18 @@
       <c r="C478" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D478" s="2">
+        <v>0</v>
+      </c>
+      <c r="E478" s="2">
+        <v>0</v>
+      </c>
+      <c r="F478" s="3">
+        <v>0</v>
+      </c>
+      <c r="G478">
+        <v>-118</v>
+      </c>
       <c r="H478" t="s">
         <v>14</v>
       </c>
@@ -13347,6 +14489,18 @@
       <c r="C479" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D479" s="2">
+        <v>0</v>
+      </c>
+      <c r="E479" s="2">
+        <v>0</v>
+      </c>
+      <c r="F479" s="3">
+        <v>0</v>
+      </c>
+      <c r="G479">
+        <v>-118</v>
+      </c>
       <c r="H479" t="s">
         <v>14</v>
       </c>
@@ -13413,6 +14567,18 @@
       <c r="C482" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D482" s="2">
+        <v>0</v>
+      </c>
+      <c r="E482" s="2">
+        <v>0</v>
+      </c>
+      <c r="F482" s="3">
+        <v>0</v>
+      </c>
+      <c r="G482">
+        <v>-122</v>
+      </c>
       <c r="H482" t="s">
         <v>14</v>
       </c>
@@ -13427,6 +14593,18 @@
       <c r="C483" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D483" s="2">
+        <v>0</v>
+      </c>
+      <c r="E483" s="2">
+        <v>0</v>
+      </c>
+      <c r="F483" s="3">
+        <v>0</v>
+      </c>
+      <c r="G483">
+        <v>-122</v>
+      </c>
       <c r="H483" t="s">
         <v>14</v>
       </c>
@@ -13779,6 +14957,18 @@
       <c r="C497" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D497" s="2">
+        <v>0</v>
+      </c>
+      <c r="E497" s="2">
+        <v>0</v>
+      </c>
+      <c r="F497" s="3">
+        <v>0</v>
+      </c>
+      <c r="G497">
+        <v>-131</v>
+      </c>
       <c r="H497" t="s">
         <v>14</v>
       </c>
@@ -13819,6 +15009,18 @@
       <c r="C499" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D499" s="2">
+        <v>0</v>
+      </c>
+      <c r="E499" s="2">
+        <v>0</v>
+      </c>
+      <c r="F499" s="3">
+        <v>0</v>
+      </c>
+      <c r="G499">
+        <v>-131</v>
+      </c>
       <c r="H499" t="s">
         <v>14</v>
       </c>
@@ -14145,9 +15347,18 @@
       <c r="C512" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D512" s="2"/>
-      <c r="E512" s="2"/>
-      <c r="F512" s="1"/>
+      <c r="D512" s="2">
+        <v>0</v>
+      </c>
+      <c r="E512" s="2">
+        <v>0</v>
+      </c>
+      <c r="F512" s="3">
+        <v>0</v>
+      </c>
+      <c r="G512">
+        <v>-235</v>
+      </c>
       <c r="H512" t="s">
         <v>14</v>
       </c>
@@ -14292,6 +15503,18 @@
       <c r="C518" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D518" s="2">
+        <v>0</v>
+      </c>
+      <c r="E518" s="2">
+        <v>0</v>
+      </c>
+      <c r="F518" s="3">
+        <v>0</v>
+      </c>
+      <c r="G518">
+        <v>-238</v>
+      </c>
       <c r="H518" t="s">
         <v>14</v>
       </c>
@@ -15138,9 +16361,18 @@
       <c r="C551" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D551" s="2"/>
-      <c r="E551" s="2"/>
-      <c r="F551" s="1"/>
+      <c r="D551" s="2">
+        <v>0</v>
+      </c>
+      <c r="E551" s="2">
+        <v>0</v>
+      </c>
+      <c r="F551" s="3">
+        <v>0</v>
+      </c>
+      <c r="G551">
+        <v>-291</v>
+      </c>
       <c r="H551" t="s">
         <v>14</v>
       </c>
@@ -16299,6 +17531,18 @@
       <c r="C596" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D596" s="2">
+        <v>0</v>
+      </c>
+      <c r="E596" s="2">
+        <v>0</v>
+      </c>
+      <c r="F596" s="3">
+        <v>0</v>
+      </c>
+      <c r="G596">
+        <v>-185</v>
+      </c>
       <c r="H596" t="s">
         <v>14</v>
       </c>
@@ -16417,6 +17661,18 @@
       <c r="C601" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D601" s="2">
+        <v>0</v>
+      </c>
+      <c r="E601" s="2">
+        <v>0</v>
+      </c>
+      <c r="F601" s="3">
+        <v>0</v>
+      </c>
+      <c r="G601">
+        <v>-188</v>
+      </c>
       <c r="H601" t="s">
         <v>14</v>
       </c>
@@ -17107,6 +18363,18 @@
       <c r="C628" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D628" s="2">
+        <v>0</v>
+      </c>
+      <c r="E628" s="2">
+        <v>0</v>
+      </c>
+      <c r="F628" s="3">
+        <v>0</v>
+      </c>
+      <c r="G628">
+        <v>-219</v>
+      </c>
       <c r="H628" t="s">
         <v>14</v>
       </c>
@@ -17433,9 +18701,18 @@
       <c r="C641" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D641" s="2"/>
-      <c r="E641" s="2"/>
-      <c r="F641" s="1"/>
+      <c r="D641" s="2">
+        <v>0</v>
+      </c>
+      <c r="E641" s="2">
+        <v>0</v>
+      </c>
+      <c r="F641" s="3">
+        <v>0</v>
+      </c>
+      <c r="G641">
+        <v>-320</v>
+      </c>
       <c r="H641" t="s">
         <v>14</v>
       </c>
@@ -17528,6 +18805,18 @@
       <c r="C645" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D645" s="2">
+        <v>0</v>
+      </c>
+      <c r="E645" s="2">
+        <v>0</v>
+      </c>
+      <c r="F645" s="3">
+        <v>0</v>
+      </c>
+      <c r="G645">
+        <v>-322</v>
+      </c>
       <c r="H645" t="s">
         <v>14</v>
       </c>
@@ -17568,6 +18857,18 @@
       <c r="C647" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D647" s="2">
+        <v>0</v>
+      </c>
+      <c r="E647" s="2">
+        <v>0</v>
+      </c>
+      <c r="F647" s="3">
+        <v>0</v>
+      </c>
+      <c r="G647">
+        <v>-322</v>
+      </c>
       <c r="H647" t="s">
         <v>14</v>
       </c>
@@ -17581,6 +18882,18 @@
       </c>
       <c r="C648" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="D648" s="2">
+        <v>0</v>
+      </c>
+      <c r="E648" s="2">
+        <v>0</v>
+      </c>
+      <c r="F648" s="3">
+        <v>0</v>
+      </c>
+      <c r="G648">
+        <v>-322</v>
       </c>
       <c r="H648" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
fix SB LED 4 and small changes
</commit_message>
<xml_diff>
--- a/led_locations.xlsx
+++ b/led_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BF8B0-7E4B-46C2-A398-77C74AA4563E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900148D5-3A6F-4FE3-9F78-61A00A172172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19215" yWindow="15" windowWidth="19185" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2032,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H653"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="D209" sqref="D209"/>
+    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="E331" sqref="E331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10638,11 +10638,11 @@
       <c r="C331" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D331">
-        <v>43.431989999999999</v>
-      </c>
-      <c r="E331">
-        <v>-119.89362199999999</v>
+      <c r="D331" s="2">
+        <v>34.432329000000003</v>
+      </c>
+      <c r="E331" s="2">
+        <v>-119.886923</v>
       </c>
       <c r="F331" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
refactor leds 329/330 and small fixes
</commit_message>
<xml_diff>
--- a/led_locations.xlsx
+++ b/led_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900148D5-3A6F-4FE3-9F78-61A00A172172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960895F8-A7BA-4290-96AB-32FA11695CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19215" yWindow="15" windowWidth="19185" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2032,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H653"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
-      <selection activeCell="E331" sqref="E331"/>
+    <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
+      <selection activeCell="G653" sqref="G653"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5205,24 +5205,24 @@
         <v>6</v>
       </c>
       <c r="D122" s="2">
-        <v>0</v>
+        <v>34.040809000000003</v>
       </c>
       <c r="E122" s="2">
-        <v>0</v>
-      </c>
-      <c r="F122" s="3">
-        <v>0</v>
+        <v>-118.88845499999999</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="G122">
-        <v>-87</v>
+        <v>54</v>
       </c>
       <c r="H122" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>188</v>
@@ -5231,24 +5231,24 @@
         <v>6</v>
       </c>
       <c r="D123" s="2">
-        <v>34.040809000000003</v>
+        <v>0</v>
       </c>
       <c r="E123" s="2">
-        <v>-118.88845499999999</v>
-      </c>
-      <c r="F123" s="1" t="s">
-        <v>208</v>
+        <v>0</v>
+      </c>
+      <c r="F123" s="3">
+        <v>0</v>
       </c>
       <c r="G123">
-        <v>54</v>
+        <v>-88</v>
       </c>
       <c r="H123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>188</v>
@@ -6444,7 +6444,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>188</v>
@@ -6470,7 +6470,7 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>188</v>
@@ -6488,7 +6488,7 @@
         <v>0</v>
       </c>
       <c r="G171">
-        <v>-329</v>
+        <v>-325</v>
       </c>
       <c r="H171" t="s">
         <v>14</v>
@@ -18976,7 +18976,7 @@
     </row>
     <row r="652" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A652" s="3">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B652" s="3" t="s">
         <v>188</v>
@@ -19002,7 +19002,7 @@
     </row>
     <row r="653" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A653" s="3">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B653" s="3" t="s">
         <v>188</v>
@@ -19020,7 +19020,7 @@
         <v>0</v>
       </c>
       <c r="G653">
-        <v>-329</v>
+        <v>-325</v>
       </c>
       <c r="H653" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
fix duplicate led reference: south 26
</commit_message>
<xml_diff>
--- a/led_locations.xlsx
+++ b/led_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960895F8-A7BA-4290-96AB-32FA11695CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232D2948-29CC-4733-A973-533EE2EB92D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2032,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H653"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A612" workbookViewId="0">
-      <selection activeCell="G653" sqref="G653"/>
+    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
+      <selection activeCell="N361" sqref="N361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11220,7 +11220,7 @@
         <v>0</v>
       </c>
       <c r="G353">
-        <v>-26</v>
+        <v>-25</v>
       </c>
       <c r="H353" t="s">
         <v>14</v>

</xml_diff>